<commit_message>
Se corrige error no carga correctamente la receta (valores arriba de 255) Se agrega mostrar texto en los botones.
</commit_message>
<xml_diff>
--- a/Diagramas/entradas y salidas plc.xlsx
+++ b/Diagramas/entradas y salidas plc.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HH\lavadora-net\trunk\Diagramas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="18795" windowHeight="8445"/>
   </bookViews>
@@ -254,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -277,11 +272,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,8 +331,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -362,7 +400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,7 +435,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -609,7 +647,7 @@
   <dimension ref="B3:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,12 +979,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
@@ -979,6 +1017,7 @@
     <mergeCell ref="B21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>